<commit_message>
Added Placing order in Zebu
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,60 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\PycharmProjects\zebu\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Script</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Target</t>
-  </si>
-  <si>
-    <t>StopLoss</t>
-  </si>
-  <si>
-    <t>Entry</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+  </numFmts>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -72,22 +47,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -353,36 +320,220 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col width="10.42578125" bestFit="1" customWidth="1" min="1" max="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Script</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Entry</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Target</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>StopLoss</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>44053</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>NIFTY</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>11257.55</v>
+      </c>
+      <c r="E2" t="n">
+        <v>11207.2</v>
+      </c>
+      <c r="F2" t="n">
+        <v>11307.9</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>44053</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>NIFTY</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>11257.55</v>
+      </c>
+      <c r="E3" t="n">
+        <v>11207.2</v>
+      </c>
+      <c r="F3" t="n">
+        <v>11307.9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>44053</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>NIFTY</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>11257.55</v>
+      </c>
+      <c r="E4" t="n">
+        <v>11207.2</v>
+      </c>
+      <c r="F4" t="n">
+        <v>11307.9</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>44053</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>NIFTY</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>11257.55</v>
+      </c>
+      <c r="E5" t="n">
+        <v>11207.2</v>
+      </c>
+      <c r="F5" t="n">
+        <v>11307.9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>44053</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>NIFTY</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>11257.55</v>
+      </c>
+      <c r="E6" t="n">
+        <v>11207.2</v>
+      </c>
+      <c r="F6" t="n">
+        <v>11307.9</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>44053</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>NIFTY</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>11257.55</v>
+      </c>
+      <c r="E7" t="n">
+        <v>11207.2</v>
+      </c>
+      <c r="F7" t="n">
+        <v>11307.9</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>44053</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>NIFTY</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>11257.55</v>
+      </c>
+      <c r="E8" t="n">
+        <v>11207.2</v>
+      </c>
+      <c r="F8" t="n">
+        <v>11307.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added impulse 5 min strategy
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,63 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\PycharmProjects\MYAliceZebu\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Script</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Entry</t>
-  </si>
-  <si>
-    <t>Target</t>
-  </si>
-  <si>
-    <t>StopLoss</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -75,23 +48,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -357,61 +322,101 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H9" sqref="A2:H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col width="10.42578125" bestFit="1" customWidth="1" min="1" max="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Script</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Entry</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Target</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>StopLoss</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
+        <v>44056</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>NIFTY</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>11350.55</v>
+      </c>
+      <c r="E10" t="n">
+        <v>11339.9</v>
+      </c>
+      <c r="F10" t="n">
+        <v>11361.2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>